<commit_message>
Implementing WTW, and preliminary results
</commit_message>
<xml_diff>
--- a/Results/OTW/Percentages_Nocturne.xlsx
+++ b/Results/OTW/Percentages_Nocturne.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,13 +452,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>0.99</v>
+        <v>0.03</v>
       </c>
       <c r="D4" s="2">
-        <v>21.58</v>
+        <v>32.479999999999997</v>
       </c>
       <c r="E4" s="2">
-        <v>17.940000000000001</v>
+        <v>38.92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -469,13 +469,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>30.46</v>
+        <v>41.17</v>
       </c>
       <c r="D5" s="1">
-        <v>0.99</v>
+        <v>0.03</v>
       </c>
       <c r="E5" s="2">
-        <v>23.33</v>
+        <v>57.56</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -483,13 +483,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>24.77</v>
+        <v>33.94</v>
       </c>
       <c r="D6" s="2">
-        <v>18.670000000000002</v>
+        <v>67.52</v>
       </c>
       <c r="E6" s="1">
-        <v>0.99</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -532,15 +532,15 @@
       </c>
       <c r="C11" s="1">
         <f>100-C4</f>
-        <v>99.01</v>
+        <v>99.97</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ref="D11:E11" si="0">100-D4</f>
-        <v>78.42</v>
+        <v>67.52000000000001</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>82.06</v>
+        <v>61.08</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -552,15 +552,15 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ref="C12:E12" si="1">100-C5</f>
-        <v>69.539999999999992</v>
+        <v>58.83</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>99.01</v>
+        <v>99.97</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
-        <v>76.67</v>
+        <v>42.44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -569,15 +569,15 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ref="C13:E13" si="2">100-C6</f>
-        <v>75.23</v>
+        <v>66.06</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="2"/>
-        <v>81.33</v>
+        <v>32.480000000000004</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>99.01</v>
+        <v>99.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>